<commit_message>
Update to all Western species, add percent consumed data and western white pine data, update Table S1.
</commit_message>
<xml_diff>
--- a/data/raw data/FlammabilityData.xlsx
+++ b/data/raw data/FlammabilityData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27729"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20500" windowHeight="15640" activeTab="1"/>
+    <workbookView xWindow="1120" yWindow="1120" windowWidth="24480" windowHeight="13600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="61">
   <si>
     <t>Species</t>
   </si>
@@ -200,6 +200,12 @@
   </si>
   <si>
     <t>Pinus attenuata</t>
+  </si>
+  <si>
+    <t>PIMO</t>
+  </si>
+  <si>
+    <t>Pinus monticola</t>
   </si>
 </sst>
 </file>
@@ -209,7 +215,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,6 +227,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -243,8 +265,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -252,7 +278,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -523,7 +553,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -601,10 +631,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -912,45 +942,45 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>11</v>
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
+        <v>60</v>
       </c>
       <c r="C14" s="1">
-        <v>77</v>
+        <v>75.14</v>
       </c>
       <c r="D14" s="1">
-        <v>79.7</v>
+        <v>90.29</v>
       </c>
       <c r="E14" s="1">
-        <v>136.9</v>
+        <v>391.43</v>
       </c>
       <c r="F14" s="1">
-        <v>92</v>
+        <v>82.78</v>
       </c>
       <c r="G14" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" t="s">
-        <v>13</v>
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C15" s="1">
-        <v>67.3</v>
+        <v>77</v>
       </c>
       <c r="D15" s="1">
-        <v>63.5</v>
+        <v>79.7</v>
       </c>
       <c r="E15" s="1">
-        <v>360.1</v>
+        <v>136.9</v>
       </c>
       <c r="F15" s="1">
-        <v>81.400000000000006</v>
+        <v>92</v>
       </c>
       <c r="G15" t="s">
         <v>10</v>
@@ -958,45 +988,45 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="C16" s="1">
-        <v>76.142857142857139</v>
+        <v>67.3</v>
       </c>
       <c r="D16" s="1">
-        <v>75.714285714285708</v>
+        <v>63.5</v>
       </c>
       <c r="E16" s="1">
-        <v>327.85714285714283</v>
+        <v>360.1</v>
       </c>
       <c r="F16" s="1">
-        <v>88.8</v>
+        <v>81.400000000000006</v>
       </c>
       <c r="G16" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1">
-        <v>84.857142857142861</v>
+        <v>76.142857142857139</v>
       </c>
       <c r="D17" s="1">
-        <v>57.714285714285715</v>
+        <v>75.714285714285708</v>
       </c>
       <c r="E17" s="1">
-        <v>495</v>
+        <v>327.85714285714283</v>
       </c>
       <c r="F17" s="1">
-        <v>91.4</v>
+        <v>88.8</v>
       </c>
       <c r="G17" t="s">
         <v>34</v>
@@ -1004,45 +1034,45 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C18" s="1">
-        <v>26.2</v>
+        <v>84.857142857142861</v>
       </c>
       <c r="D18" s="1">
-        <v>105.8</v>
+        <v>57.714285714285715</v>
       </c>
       <c r="E18" s="1">
-        <v>21.8</v>
+        <v>495</v>
       </c>
       <c r="F18" s="1">
-        <v>26.6</v>
+        <v>91.4</v>
       </c>
       <c r="G18" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C19" s="1">
-        <v>42.6</v>
+        <v>26.2</v>
       </c>
       <c r="D19" s="1">
-        <v>148.5</v>
+        <v>105.8</v>
       </c>
       <c r="E19" s="1">
-        <v>242.6</v>
+        <v>21.8</v>
       </c>
       <c r="F19" s="1">
-        <v>75.8</v>
+        <v>26.6</v>
       </c>
       <c r="G19" t="s">
         <v>14</v>
@@ -1050,22 +1080,22 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C20" s="1">
-        <v>59.4</v>
+        <v>42.6</v>
       </c>
       <c r="D20" s="1">
-        <v>73.400000000000006</v>
+        <v>148.5</v>
       </c>
       <c r="E20" s="1">
-        <v>317.3</v>
+        <v>242.6</v>
       </c>
       <c r="F20" s="1">
-        <v>86.1</v>
+        <v>75.8</v>
       </c>
       <c r="G20" t="s">
         <v>14</v>
@@ -1073,22 +1103,22 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C21" s="1">
-        <v>42.4</v>
+        <v>59.4</v>
       </c>
       <c r="D21" s="1">
-        <v>113.2</v>
+        <v>73.400000000000006</v>
       </c>
       <c r="E21" s="1">
-        <v>130.69999999999999</v>
+        <v>317.3</v>
       </c>
       <c r="F21" s="1">
-        <v>45.7</v>
+        <v>86.1</v>
       </c>
       <c r="G21" t="s">
         <v>14</v>
@@ -1096,24 +1126,47 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="1">
+        <v>42.4</v>
+      </c>
+      <c r="D22" s="1">
+        <v>113.2</v>
+      </c>
+      <c r="E22" s="1">
+        <v>130.69999999999999</v>
+      </c>
+      <c r="F22" s="1">
+        <v>45.7</v>
+      </c>
+      <c r="G22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
         <v>28</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C23" s="1">
         <v>24.6</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D23" s="1">
         <v>68.400000000000006</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E23" s="1">
         <v>43.6</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F23" s="1">
         <v>18.8</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G23" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>